<commit_message>
update region6 in province_simplify
</commit_message>
<xml_diff>
--- a/province/province_simplify.xlsx
+++ b/province/province_simplify.xlsx
@@ -466,12 +466,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>DESTINATIO</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>REGION6</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>DESTINATION</t>
         </is>
       </c>
     </row>
@@ -508,12 +508,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -550,12 +550,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -592,12 +592,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -634,12 +634,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -676,12 +676,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -718,12 +718,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -760,12 +760,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -802,12 +802,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -844,12 +844,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>ภาคกลาง</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -928,12 +928,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>ภาคตะวันออก</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -970,12 +970,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
           <t>ภาคตะวันออก</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -1012,12 +1012,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
           <t>ภาคตะวันออก</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1054,12 +1054,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>ภาคตะวันออก</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1096,12 +1096,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
           <t>ภาคตะวันออก</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
           <t>ภาคตะวันออก</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1180,12 +1180,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>ภาคตะวันออก</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -1222,12 +1222,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
           <t>ภาคตะวันออก</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1264,12 +1264,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -1306,12 +1306,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1348,12 +1348,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1390,12 +1390,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1432,12 +1432,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1474,12 +1474,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1516,12 +1516,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1558,12 +1558,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1600,12 +1600,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1642,12 +1642,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1684,12 +1684,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -1726,12 +1726,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1768,12 +1768,12 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1810,12 +1810,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1852,12 +1852,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1894,12 +1894,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1936,12 +1936,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -1978,12 +1978,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2020,12 +2020,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2062,12 +2062,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
           <t>ภาคตะวันออกเฉียงเหนือ</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2104,12 +2104,12 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -2146,12 +2146,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2188,12 +2188,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2230,12 +2230,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2272,12 +2272,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2314,12 +2314,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2356,12 +2356,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2398,12 +2398,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2440,12 +2440,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
           <t>ภาคเหนือ</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2482,12 +2482,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2524,12 +2524,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2566,12 +2566,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2608,12 +2608,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคตะวันตก</t>
         </is>
       </c>
     </row>
@@ -2650,12 +2650,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2692,12 +2692,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2734,12 +2734,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2776,12 +2776,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>ภาคเหนือ</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2818,12 +2818,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
           <t>ภาคตะวันตก</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2860,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
           <t>ภาคตะวันตก</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -2902,12 +2902,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>ภาคตะวันตก</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2944,12 +2944,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>ภาคตะวันตก</t>
+          <t>เมืองหลัก</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>เมืองหลัก</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -2986,12 +2986,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>ภาคตะวันตก</t>
+          <t>เมืองหลัก</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>เมืองหลัก</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -3028,12 +3028,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>ภาคตะวันตก</t>
+          <t>เมืองรอง</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>เมืองรอง</t>
+          <t>ภาคกลาง</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
           <t>ภาคตะวันตก</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -3112,12 +3112,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
           <t>ภาคตะวันตก</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -3154,12 +3154,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3196,12 +3196,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -3238,12 +3238,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -3322,12 +3322,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -3364,12 +3364,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3406,12 +3406,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3448,12 +3448,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
+          <t>เมืองหลัก</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>เมืองหลัก</t>
         </is>
       </c>
     </row>
@@ -3490,12 +3490,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3532,12 +3532,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3574,12 +3574,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3616,12 +3616,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3658,12 +3658,12 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>
@@ -3700,12 +3700,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
+          <t>เมืองรอง</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
           <t>ภาคใต้</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>เมืองรอง</t>
         </is>
       </c>
     </row>

</xml_diff>